<commit_message>
Updated parts list - more bypass capacitors and higher voltage rating
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -66,9 +66,6 @@
     <t>INA2141U</t>
   </si>
   <si>
-    <t>C5-C6</t>
-  </si>
-  <si>
     <t>Bypass capacitor for instrumation amplifier</t>
   </si>
   <si>
@@ -114,15 +111,9 @@
     <t>0805, 10k, 1%, 1/8W</t>
   </si>
   <si>
-    <t>0402, Ceramic, X5R, 0.47uF, 10%, 6.3V</t>
-  </si>
-  <si>
     <t>GRM155R60J474KE19D</t>
   </si>
   <si>
-    <t>http://www.digikey.com/short/3t3q8z</t>
-  </si>
-  <si>
     <t>0402, Ceramic, X7R, 0.1uF, 10%, 25V</t>
   </si>
   <si>
@@ -261,10 +252,19 @@
     <t xml:space="preserve">1658620-3 </t>
   </si>
   <si>
-    <t>http://www.digikey.com/short/3t4q8m</t>
-  </si>
-  <si>
     <t>Digikey cart</t>
+  </si>
+  <si>
+    <t>C5-C10</t>
+  </si>
+  <si>
+    <t>0402, Ceramic, X5R, 0.47uF, 10%, 10V</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/short/3tbjbm</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/short/3tbj5t</t>
   </si>
 </sst>
 </file>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -643,13 +643,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
         <v>81</v>
-      </c>
-      <c r="J1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -663,16 +663,16 @@
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -686,202 +686,202 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
         <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
         <v>60</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>59</v>
-      </c>
-      <c r="E9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
         <v>66</v>
-      </c>
-      <c r="D11" t="s">
-        <v>69</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -899,7 +899,7 @@
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -910,19 +910,19 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -933,19 +933,19 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" t="s">
         <v>72</v>
-      </c>
-      <c r="E14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -956,19 +956,19 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>